<commit_message>
Enable new VBF seeds
</commit_message>
<xml_diff>
--- a/official/L1Menu_Collisions2023_v1_1_0/PrescaleTable/L1Menu_Collisions2023_v1_1_0.xlsx
+++ b/official/L1Menu_Collisions2023_v1_1_0/PrescaleTable/L1Menu_Collisions2023_v1_1_0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/L1MenuRun3-master 16/development/L1Menu_Collisions2023_v1_1_0/PrescaleTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/L1MenuRun3-oggi/official/L1Menu_Collisions2023_v1_1_0/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DE169A-3480-EF43-B731-58EA5E6ABF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4EBEAF2-1F57-4347-A000-3F10B1439590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15280" yWindow="-19260" windowWidth="25600" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1790,10 +1790,10 @@
   <dimension ref="A1:AD1023"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P381" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C312" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W407" sqref="W407"/>
+      <selection pane="bottomRight" activeCell="H330" sqref="H330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -26239,64 +26239,64 @@
         <v>0</v>
       </c>
       <c r="D331" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E331" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F331" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G331" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H331" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I331" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J331" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K331" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L331" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M331" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N331" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O331" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P331" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q331" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R331" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S331" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T331" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U331" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V331" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W331" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X331" s="5">
         <v>0</v>
@@ -26313,64 +26313,64 @@
         <v>0</v>
       </c>
       <c r="D332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X332" s="5">
         <v>0</v>
@@ -26387,64 +26387,64 @@
         <v>0</v>
       </c>
       <c r="D333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X333" s="5">
         <v>0</v>
@@ -26461,64 +26461,64 @@
         <v>0</v>
       </c>
       <c r="D334" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E334" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F334" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G334" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H334" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I334" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J334" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K334" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L334" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M334" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N334" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O334" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P334" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q334" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R334" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S334" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T334" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U334" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V334" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W334" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X334" s="5">
         <v>0</v>
@@ -47872,7 +47872,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:X251 D253:X360 D364:X430">
+  <conditionalFormatting sqref="D2:X251 D364:X430 D253:X360">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>